<commit_message>
Tested different network topologies
</commit_message>
<xml_diff>
--- a/biases.xlsx
+++ b/biases.xlsx
@@ -366,7 +366,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B2:B13"/>
+  <dimension ref="B2:B301"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -376,62 +376,1502 @@
   <sheetData>
     <row r="2">
       <c r="B2" t="n">
-        <v>-3.354670763355224</v>
+        <v>0.5632220301049876</v>
       </c>
     </row>
     <row r="3">
       <c r="B3" t="n">
-        <v>9.635604431468609</v>
+        <v>-0.6230956463129097</v>
       </c>
     </row>
     <row r="4">
       <c r="B4" t="n">
-        <v>-12.70644129660954</v>
+        <v>-1.108682112660156</v>
       </c>
     </row>
     <row r="5">
       <c r="B5" t="n">
-        <v>6.607161497027612</v>
+        <v>-0.4015393396356507</v>
       </c>
     </row>
     <row r="6">
       <c r="B6" t="n">
-        <v>11.74756403140076</v>
+        <v>0.3884724284871733</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" t="n">
-        <v>-0.7237842378156424</v>
+        <v>0.6682850667984307</v>
       </c>
     </row>
     <row r="8">
       <c r="B8" t="n">
-        <v>-16.13259796652465</v>
+        <v>-0.6031501835064531</v>
       </c>
     </row>
     <row r="9">
       <c r="B9" t="n">
-        <v>-4.036394218969259</v>
+        <v>0.05638232932328398</v>
       </c>
     </row>
     <row r="10">
       <c r="B10" t="n">
-        <v>16.00519155458776</v>
+        <v>-1.18494470550335</v>
       </c>
     </row>
     <row r="11">
       <c r="B11" t="n">
-        <v>-5.475953582842701</v>
+        <v>0.957776272099977</v>
       </c>
     </row>
     <row r="12">
       <c r="B12" t="n">
-        <v>3.780674163209742</v>
+        <v>-0.4856009529941491</v>
       </c>
     </row>
     <row r="13">
       <c r="B13" t="n">
-        <v>-2.997914908683567</v>
+        <v>-0.4839304666215388</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="B14" t="n">
+        <v>-0.5439097847916556</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="B15" t="n">
+        <v>-0.2516036843627684</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="B16" t="n">
+        <v>-0.606671181268858</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="B17" t="n">
+        <v>0.4010512631750461</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="B18" t="n">
+        <v>0.7633660325150232</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="B19" t="n">
+        <v>-0.2702035221130272</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="B20" t="n">
+        <v>0.8917129006334474</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="B21" t="n">
+        <v>0.1778220742146587</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="B22" t="n">
+        <v>-0.547710292631825</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="B23" t="n">
+        <v>-0.8587331496553781</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="B24" t="n">
+        <v>0.6591748990440396</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="B25" t="n">
+        <v>-0.2848739739617682</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="B26" t="n">
+        <v>0.8401585238738195</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="B27" t="n">
+        <v>-1.494344240582467</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="B28" t="n">
+        <v>0.461637077541478</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="B29" t="n">
+        <v>-0.5697324076887639</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="B30" t="n">
+        <v>0.1025676376982908</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="B31" t="n">
+        <v>0.1095193192487071</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="B32" t="n">
+        <v>-0.9438310671740363</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="B33" t="n">
+        <v>-0.9031783084038753</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="B34" t="n">
+        <v>0.2653104789841195</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="B35" t="n">
+        <v>-1.052533485880829</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="B36" t="n">
+        <v>0.5940229815870279</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="B37" t="n">
+        <v>-0.558764043410972</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="B38" t="n">
+        <v>1.310398430899509</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="B39" t="n">
+        <v>-0.516954843843671</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="B40" t="n">
+        <v>-1.068599931012401</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="B41" t="n">
+        <v>0.4319861707225781</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="B42" t="n">
+        <v>0.06087109619504057</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="B43" t="n">
+        <v>0.02924582951369955</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="B44" t="n">
+        <v>-0.1634747344427083</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="B45" t="n">
+        <v>0.6855754891098584</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="B46" t="n">
+        <v>0.3568329751854707</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="B47" t="n">
+        <v>1.320287733429097</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="B48" t="n">
+        <v>-0.668344159839545</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="B49" t="n">
+        <v>0.8256901231807203</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="B50" t="n">
+        <v>-0.4277975261426529</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="B51" t="n">
+        <v>0.2235360244150649</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="B52" t="n">
+        <v>-0.4205840899927755</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="B53" t="n">
+        <v>-0.2990658534362</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="B54" t="n">
+        <v>-0.8161156141080915</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="B55" t="n">
+        <v>0.04707750178636412</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="B56" t="n">
+        <v>0.08412556661198305</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="B57" t="n">
+        <v>1.627091615310499</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="B58" t="n">
+        <v>0.3880563293658141</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="B59" t="n">
+        <v>0.2111841133584153</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="B60" t="n">
+        <v>-0.461056334059407</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="B61" t="n">
+        <v>0.4888688832497634</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="B62" t="n">
+        <v>0.9690332707526447</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="B63" t="n">
+        <v>0.01023709525153655</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="B64" t="n">
+        <v>0.745689279082171</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="B65" t="n">
+        <v>-0.5644709525632048</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="B66" t="n">
+        <v>-0.4655002949692663</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="B67" t="n">
+        <v>0.1238691038663635</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="B68" t="n">
+        <v>0.8201311193236792</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="B69" t="n">
+        <v>-0.0009567446190965412</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="B70" t="n">
+        <v>-0.09794070018406938</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="B71" t="n">
+        <v>0.07845011914530955</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="B72" t="n">
+        <v>-0.1663440392441525</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="B73" t="n">
+        <v>0.2764208689531379</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="B74" t="n">
+        <v>-0.3721123581018822</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="B75" t="n">
+        <v>0.3672164568383231</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="B76" t="n">
+        <v>0.4438193003508602</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="B77" t="n">
+        <v>1.081383077538022</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="B78" t="n">
+        <v>0.5519493117017279</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="B79" t="n">
+        <v>-0.5668900449368943</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="B80" t="n">
+        <v>0.1445989020037367</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="B81" t="n">
+        <v>-0.09571732858906896</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="B82" t="n">
+        <v>1.287594002723901</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="B83" t="n">
+        <v>0.2531351871026027</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="B84" t="n">
+        <v>-0.8542792160299482</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="B85" t="n">
+        <v>0.01081388553643773</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="B86" t="n">
+        <v>-1.21223855069382</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="B87" t="n">
+        <v>-1.063520596669004</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="B88" t="n">
+        <v>-0.8827771616640883</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="B89" t="n">
+        <v>-0.7719553828389339</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="B90" t="n">
+        <v>-0.4086525244909461</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="B91" t="n">
+        <v>-0.4658316414479347</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="B92" t="n">
+        <v>-0.5116954240312406</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="B93" t="n">
+        <v>1.158375467664096</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="B94" t="n">
+        <v>-0.06766454936437839</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="B95" t="n">
+        <v>0.7208920765470919</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="B96" t="n">
+        <v>-0.8983122524344328</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="B97" t="n">
+        <v>0.3530016769333183</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="B98" t="n">
+        <v>0.6569441220906999</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="B99" t="n">
+        <v>-0.1936830184034075</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="B100" t="n">
+        <v>-0.7424930160369192</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="B101" t="n">
+        <v>-0.5448472908636901</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="B102" t="n">
+        <v>-0.2550708726609501</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="B103" t="n">
+        <v>-0.05856882625093612</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="B104" t="n">
+        <v>-0.1055975181906801</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="B105" t="n">
+        <v>0.05874535978584164</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="B106" t="n">
+        <v>0.09528422496680508</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="B107" t="n">
+        <v>0.005573148209975605</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="B108" t="n">
+        <v>0.3189008683464125</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="B109" t="n">
+        <v>-0.8518481034285598</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="B110" t="n">
+        <v>0.8537593684617834</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="B111" t="n">
+        <v>1.407221080494035</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="B112" t="n">
+        <v>-0.110425113529017</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="B113" t="n">
+        <v>-0.1388787450412242</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="B114" t="n">
+        <v>0.7276619318504066</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="B115" t="n">
+        <v>-0.4717278411005988</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="B116" t="n">
+        <v>-0.04450220706958006</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="B117" t="n">
+        <v>-0.3807674719252057</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="B118" t="n">
+        <v>-0.9324412992013107</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="B119" t="n">
+        <v>-0.4941722617465982</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="B120" t="n">
+        <v>-0.540867148864103</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="B121" t="n">
+        <v>-1.035706724960068</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="B122" t="n">
+        <v>0.007362990559548792</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="B123" t="n">
+        <v>-1.071047901910546</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="B124" t="n">
+        <v>-0.3259728489676127</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="B125" t="n">
+        <v>-0.8446941042378768</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="B126" t="n">
+        <v>0.367906345402521</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="B127" t="n">
+        <v>0.5785960001242515</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="B128" t="n">
+        <v>-0.4126309546168603</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="B129" t="n">
+        <v>0.430306920306657</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="B130" t="n">
+        <v>0.358426863698289</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="B131" t="n">
+        <v>-0.05634330027739139</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="B132" t="n">
+        <v>0.6849919722619497</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="B133" t="n">
+        <v>0.6554839503763145</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="B134" t="n">
+        <v>-0.2499959919249391</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="B135" t="n">
+        <v>0.9869184470724244</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="B136" t="n">
+        <v>0.4965886795807833</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="B137" t="n">
+        <v>-0.1136856042565895</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="B138" t="n">
+        <v>-0.4362178837051577</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="B139" t="n">
+        <v>-1.16723179177712</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="B140" t="n">
+        <v>1.364617300356495</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="B141" t="n">
+        <v>-0.1830252365738974</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="B142" t="n">
+        <v>0.08857455963463956</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="B143" t="n">
+        <v>-0.5353241660265453</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="B144" t="n">
+        <v>0.8543785211360491</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="B145" t="n">
+        <v>-0.2011787271415438</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="B146" t="n">
+        <v>-0.04783334258524395</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="B147" t="n">
+        <v>0.4413582452890908</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="B148" t="n">
+        <v>0.3783204633286731</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="B149" t="n">
+        <v>0.858855042742052</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="B150" t="n">
+        <v>-0.4917783967123893</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="B151" t="n">
+        <v>0.7876347092618239</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="B152" t="n">
+        <v>-0.1550491614781375</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="B153" t="n">
+        <v>0.7687626341950977</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="B154" t="n">
+        <v>-0.4698818520746445</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="B155" t="n">
+        <v>0.5629932753534895</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="B156" t="n">
+        <v>0.4126909235233646</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="B157" t="n">
+        <v>0.4393734075690512</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="B158" t="n">
+        <v>0.8272823108931049</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="B159" t="n">
+        <v>-0.5527585256179735</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="B160" t="n">
+        <v>0.6408015342251671</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="B161" t="n">
+        <v>0.1689097537887874</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="B162" t="n">
+        <v>0.9488974574151428</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="B163" t="n">
+        <v>0.3495753820730556</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="B164" t="n">
+        <v>1.166052063348669</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="B165" t="n">
+        <v>1.159607296733532</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="B166" t="n">
+        <v>0.0107759640328639</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="B167" t="n">
+        <v>0.6097195852865054</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="B168" t="n">
+        <v>-0.2566251682855704</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="B169" t="n">
+        <v>-0.371651026188347</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="B170" t="n">
+        <v>1.345073574776163</v>
+      </c>
+    </row>
+    <row r="171">
+      <c r="B171" t="n">
+        <v>-0.3967354315092764</v>
+      </c>
+    </row>
+    <row r="172">
+      <c r="B172" t="n">
+        <v>0.8642451024734535</v>
+      </c>
+    </row>
+    <row r="173">
+      <c r="B173" t="n">
+        <v>0.1500806648913364</v>
+      </c>
+    </row>
+    <row r="174">
+      <c r="B174" t="n">
+        <v>0.5104343906577588</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="B175" t="n">
+        <v>0.4789219931866668</v>
+      </c>
+    </row>
+    <row r="176">
+      <c r="B176" t="n">
+        <v>-0.6205369481179338</v>
+      </c>
+    </row>
+    <row r="177">
+      <c r="B177" t="n">
+        <v>-0.3987507028686603</v>
+      </c>
+    </row>
+    <row r="178">
+      <c r="B178" t="n">
+        <v>-0.2325026852814345</v>
+      </c>
+    </row>
+    <row r="179">
+      <c r="B179" t="n">
+        <v>-0.3104259550485555</v>
+      </c>
+    </row>
+    <row r="180">
+      <c r="B180" t="n">
+        <v>-0.990733985738569</v>
+      </c>
+    </row>
+    <row r="181">
+      <c r="B181" t="n">
+        <v>-0.6370697671618187</v>
+      </c>
+    </row>
+    <row r="182">
+      <c r="B182" t="n">
+        <v>-0.1161580984545754</v>
+      </c>
+    </row>
+    <row r="183">
+      <c r="B183" t="n">
+        <v>0.08678469104196891</v>
+      </c>
+    </row>
+    <row r="184">
+      <c r="B184" t="n">
+        <v>-0.3824047823745183</v>
+      </c>
+    </row>
+    <row r="185">
+      <c r="B185" t="n">
+        <v>-1.19562282691527</v>
+      </c>
+    </row>
+    <row r="186">
+      <c r="B186" t="n">
+        <v>0.3569147721259073</v>
+      </c>
+    </row>
+    <row r="187">
+      <c r="B187" t="n">
+        <v>0.4611523159646314</v>
+      </c>
+    </row>
+    <row r="188">
+      <c r="B188" t="n">
+        <v>-0.009010666435478501</v>
+      </c>
+    </row>
+    <row r="189">
+      <c r="B189" t="n">
+        <v>-0.2787460447906669</v>
+      </c>
+    </row>
+    <row r="190">
+      <c r="B190" t="n">
+        <v>0.002175748324992232</v>
+      </c>
+    </row>
+    <row r="191">
+      <c r="B191" t="n">
+        <v>-0.4043677720662204</v>
+      </c>
+    </row>
+    <row r="192">
+      <c r="B192" t="n">
+        <v>1.180626766480652</v>
+      </c>
+    </row>
+    <row r="193">
+      <c r="B193" t="n">
+        <v>1.131626927445987</v>
+      </c>
+    </row>
+    <row r="194">
+      <c r="B194" t="n">
+        <v>-0.02273579937387293</v>
+      </c>
+    </row>
+    <row r="195">
+      <c r="B195" t="n">
+        <v>-0.8005416357504767</v>
+      </c>
+    </row>
+    <row r="196">
+      <c r="B196" t="n">
+        <v>-0.4364297581388295</v>
+      </c>
+    </row>
+    <row r="197">
+      <c r="B197" t="n">
+        <v>0.3520484943716702</v>
+      </c>
+    </row>
+    <row r="198">
+      <c r="B198" t="n">
+        <v>0.08637264985432071</v>
+      </c>
+    </row>
+    <row r="199">
+      <c r="B199" t="n">
+        <v>-0.7897168464471563</v>
+      </c>
+    </row>
+    <row r="200">
+      <c r="B200" t="n">
+        <v>-0.6063762596185762</v>
+      </c>
+    </row>
+    <row r="201">
+      <c r="B201" t="n">
+        <v>0.182246657472017</v>
+      </c>
+    </row>
+    <row r="202">
+      <c r="B202" t="n">
+        <v>-0.813726037966239</v>
+      </c>
+    </row>
+    <row r="203">
+      <c r="B203" t="n">
+        <v>0.5929405174659215</v>
+      </c>
+    </row>
+    <row r="204">
+      <c r="B204" t="n">
+        <v>0.3189788996087429</v>
+      </c>
+    </row>
+    <row r="205">
+      <c r="B205" t="n">
+        <v>0.1554850517777272</v>
+      </c>
+    </row>
+    <row r="206">
+      <c r="B206" t="n">
+        <v>-0.856191079612948</v>
+      </c>
+    </row>
+    <row r="207">
+      <c r="B207" t="n">
+        <v>0.1139404641100666</v>
+      </c>
+    </row>
+    <row r="208">
+      <c r="B208" t="n">
+        <v>-0.9102194265635306</v>
+      </c>
+    </row>
+    <row r="209">
+      <c r="B209" t="n">
+        <v>1.114289899666927</v>
+      </c>
+    </row>
+    <row r="210">
+      <c r="B210" t="n">
+        <v>1.716073014842424</v>
+      </c>
+    </row>
+    <row r="211">
+      <c r="B211" t="n">
+        <v>-0.5488601173305349</v>
+      </c>
+    </row>
+    <row r="212">
+      <c r="B212" t="n">
+        <v>-0.5047470979291155</v>
+      </c>
+    </row>
+    <row r="213">
+      <c r="B213" t="n">
+        <v>1.053769848768009</v>
+      </c>
+    </row>
+    <row r="214">
+      <c r="B214" t="n">
+        <v>0.5345032831622845</v>
+      </c>
+    </row>
+    <row r="215">
+      <c r="B215" t="n">
+        <v>-1.081786384610914</v>
+      </c>
+    </row>
+    <row r="216">
+      <c r="B216" t="n">
+        <v>1.195438671566373</v>
+      </c>
+    </row>
+    <row r="217">
+      <c r="B217" t="n">
+        <v>0.2288778556032452</v>
+      </c>
+    </row>
+    <row r="218">
+      <c r="B218" t="n">
+        <v>-0.373523466478806</v>
+      </c>
+    </row>
+    <row r="219">
+      <c r="B219" t="n">
+        <v>-0.6083118304396559</v>
+      </c>
+    </row>
+    <row r="220">
+      <c r="B220" t="n">
+        <v>0.3336545594878079</v>
+      </c>
+    </row>
+    <row r="221">
+      <c r="B221" t="n">
+        <v>-0.952769660484849</v>
+      </c>
+    </row>
+    <row r="222">
+      <c r="B222" t="n">
+        <v>-0.1889065265680365</v>
+      </c>
+    </row>
+    <row r="223">
+      <c r="B223" t="n">
+        <v>0.7184014561463959</v>
+      </c>
+    </row>
+    <row r="224">
+      <c r="B224" t="n">
+        <v>-0.2803425904526476</v>
+      </c>
+    </row>
+    <row r="225">
+      <c r="B225" t="n">
+        <v>-0.5435825955078034</v>
+      </c>
+    </row>
+    <row r="226">
+      <c r="B226" t="n">
+        <v>-0.7261337572530115</v>
+      </c>
+    </row>
+    <row r="227">
+      <c r="B227" t="n">
+        <v>0.1391561448573645</v>
+      </c>
+    </row>
+    <row r="228">
+      <c r="B228" t="n">
+        <v>0.08258312932618204</v>
+      </c>
+    </row>
+    <row r="229">
+      <c r="B229" t="n">
+        <v>-0.5389378233377545</v>
+      </c>
+    </row>
+    <row r="230">
+      <c r="B230" t="n">
+        <v>0.6100592952055052</v>
+      </c>
+    </row>
+    <row r="231">
+      <c r="B231" t="n">
+        <v>0.1729503336063284</v>
+      </c>
+    </row>
+    <row r="232">
+      <c r="B232" t="n">
+        <v>-0.7530683897685118</v>
+      </c>
+    </row>
+    <row r="233">
+      <c r="B233" t="n">
+        <v>0.1655874460480216</v>
+      </c>
+    </row>
+    <row r="234">
+      <c r="B234" t="n">
+        <v>0.2345578743699785</v>
+      </c>
+    </row>
+    <row r="235">
+      <c r="B235" t="n">
+        <v>0.6329659863467318</v>
+      </c>
+    </row>
+    <row r="236">
+      <c r="B236" t="n">
+        <v>-1.255507108322828</v>
+      </c>
+    </row>
+    <row r="237">
+      <c r="B237" t="n">
+        <v>-0.1157277503689745</v>
+      </c>
+    </row>
+    <row r="238">
+      <c r="B238" t="n">
+        <v>-1.156523689169282</v>
+      </c>
+    </row>
+    <row r="239">
+      <c r="B239" t="n">
+        <v>0.3907585752950524</v>
+      </c>
+    </row>
+    <row r="240">
+      <c r="B240" t="n">
+        <v>-0.1233645320448403</v>
+      </c>
+    </row>
+    <row r="241">
+      <c r="B241" t="n">
+        <v>0.6718760293366506</v>
+      </c>
+    </row>
+    <row r="242">
+      <c r="B242" t="n">
+        <v>0.759168613724336</v>
+      </c>
+    </row>
+    <row r="243">
+      <c r="B243" t="n">
+        <v>-0.5381609008543479</v>
+      </c>
+    </row>
+    <row r="244">
+      <c r="B244" t="n">
+        <v>1.184862792891914</v>
+      </c>
+    </row>
+    <row r="245">
+      <c r="B245" t="n">
+        <v>-0.1252914308122563</v>
+      </c>
+    </row>
+    <row r="246">
+      <c r="B246" t="n">
+        <v>0.9369135862542928</v>
+      </c>
+    </row>
+    <row r="247">
+      <c r="B247" t="n">
+        <v>-0.5288789405117076</v>
+      </c>
+    </row>
+    <row r="248">
+      <c r="B248" t="n">
+        <v>-0.09907694227854411</v>
+      </c>
+    </row>
+    <row r="249">
+      <c r="B249" t="n">
+        <v>-1.06519388541807</v>
+      </c>
+    </row>
+    <row r="250">
+      <c r="B250" t="n">
+        <v>-0.6941557783396892</v>
+      </c>
+    </row>
+    <row r="251">
+      <c r="B251" t="n">
+        <v>-0.1417907845081532</v>
+      </c>
+    </row>
+    <row r="252">
+      <c r="B252" t="n">
+        <v>-0.4455372448848531</v>
+      </c>
+    </row>
+    <row r="253">
+      <c r="B253" t="n">
+        <v>-0.4749589274768042</v>
+      </c>
+    </row>
+    <row r="254">
+      <c r="B254" t="n">
+        <v>0.5044645938390191</v>
+      </c>
+    </row>
+    <row r="255">
+      <c r="B255" t="n">
+        <v>0.3140686441343858</v>
+      </c>
+    </row>
+    <row r="256">
+      <c r="B256" t="n">
+        <v>-1.165124592132667</v>
+      </c>
+    </row>
+    <row r="257">
+      <c r="B257" t="n">
+        <v>-0.6531964964113045</v>
+      </c>
+    </row>
+    <row r="258">
+      <c r="B258" t="n">
+        <v>1.177885064205772</v>
+      </c>
+    </row>
+    <row r="259">
+      <c r="B259" t="n">
+        <v>0.7047241058542895</v>
+      </c>
+    </row>
+    <row r="260">
+      <c r="B260" t="n">
+        <v>-0.05453468235060534</v>
+      </c>
+    </row>
+    <row r="261">
+      <c r="B261" t="n">
+        <v>-0.2231007403190391</v>
+      </c>
+    </row>
+    <row r="262">
+      <c r="B262" t="n">
+        <v>0.4117042248751022</v>
+      </c>
+    </row>
+    <row r="263">
+      <c r="B263" t="n">
+        <v>-0.1274614725159475</v>
+      </c>
+    </row>
+    <row r="264">
+      <c r="B264" t="n">
+        <v>-0.7828221047064104</v>
+      </c>
+    </row>
+    <row r="265">
+      <c r="B265" t="n">
+        <v>0.7897459559816289</v>
+      </c>
+    </row>
+    <row r="266">
+      <c r="B266" t="n">
+        <v>-1.147884644743724</v>
+      </c>
+    </row>
+    <row r="267">
+      <c r="B267" t="n">
+        <v>-0.6342062641961732</v>
+      </c>
+    </row>
+    <row r="268">
+      <c r="B268" t="n">
+        <v>0.5768821734065894</v>
+      </c>
+    </row>
+    <row r="269">
+      <c r="B269" t="n">
+        <v>-0.4032154648605241</v>
+      </c>
+    </row>
+    <row r="270">
+      <c r="B270" t="n">
+        <v>-0.5987723482355687</v>
+      </c>
+    </row>
+    <row r="271">
+      <c r="B271" t="n">
+        <v>0.09580244899818885</v>
+      </c>
+    </row>
+    <row r="272">
+      <c r="B272" t="n">
+        <v>-1.640437215946085</v>
+      </c>
+    </row>
+    <row r="273">
+      <c r="B273" t="n">
+        <v>0.09574799060977274</v>
+      </c>
+    </row>
+    <row r="274">
+      <c r="B274" t="n">
+        <v>0.2851373971911185</v>
+      </c>
+    </row>
+    <row r="275">
+      <c r="B275" t="n">
+        <v>-0.9876160188500748</v>
+      </c>
+    </row>
+    <row r="276">
+      <c r="B276" t="n">
+        <v>0.7810231536952273</v>
+      </c>
+    </row>
+    <row r="277">
+      <c r="B277" t="n">
+        <v>-0.4886152034141965</v>
+      </c>
+    </row>
+    <row r="278">
+      <c r="B278" t="n">
+        <v>0.4746932708994026</v>
+      </c>
+    </row>
+    <row r="279">
+      <c r="B279" t="n">
+        <v>0.8332125233437592</v>
+      </c>
+    </row>
+    <row r="280">
+      <c r="B280" t="n">
+        <v>-0.6903296976122998</v>
+      </c>
+    </row>
+    <row r="281">
+      <c r="B281" t="n">
+        <v>0.2837697188418918</v>
+      </c>
+    </row>
+    <row r="282">
+      <c r="B282" t="n">
+        <v>-0.6186157095179375</v>
+      </c>
+    </row>
+    <row r="283">
+      <c r="B283" t="n">
+        <v>0.3895973459372476</v>
+      </c>
+    </row>
+    <row r="284">
+      <c r="B284" t="n">
+        <v>-0.3181417953269831</v>
+      </c>
+    </row>
+    <row r="285">
+      <c r="B285" t="n">
+        <v>-1.075184026202712</v>
+      </c>
+    </row>
+    <row r="286">
+      <c r="B286" t="n">
+        <v>1.309642277007245</v>
+      </c>
+    </row>
+    <row r="287">
+      <c r="B287" t="n">
+        <v>-0.4462999138302156</v>
+      </c>
+    </row>
+    <row r="288">
+      <c r="B288" t="n">
+        <v>-1.08184599354013</v>
+      </c>
+    </row>
+    <row r="289">
+      <c r="B289" t="n">
+        <v>-0.7386549757475132</v>
+      </c>
+    </row>
+    <row r="290">
+      <c r="B290" t="n">
+        <v>-0.4559053144029017</v>
+      </c>
+    </row>
+    <row r="291">
+      <c r="B291" t="n">
+        <v>1.094728389121061</v>
+      </c>
+    </row>
+    <row r="292">
+      <c r="B292" t="n">
+        <v>0.6060925861683281</v>
+      </c>
+    </row>
+    <row r="293">
+      <c r="B293" t="n">
+        <v>0.5769709685763482</v>
+      </c>
+    </row>
+    <row r="294">
+      <c r="B294" t="n">
+        <v>-0.6350568880118183</v>
+      </c>
+    </row>
+    <row r="295">
+      <c r="B295" t="n">
+        <v>-0.6546710426732683</v>
+      </c>
+    </row>
+    <row r="296">
+      <c r="B296" t="n">
+        <v>0.7256727380093539</v>
+      </c>
+    </row>
+    <row r="297">
+      <c r="B297" t="n">
+        <v>0.3146189655641585</v>
+      </c>
+    </row>
+    <row r="298">
+      <c r="B298" t="n">
+        <v>0.1225056582343828</v>
+      </c>
+    </row>
+    <row r="299">
+      <c r="B299" t="n">
+        <v>-0.3651203418081353</v>
+      </c>
+    </row>
+    <row r="300">
+      <c r="B300" t="n">
+        <v>0.3112384739313558</v>
+      </c>
+    </row>
+    <row r="301">
+      <c r="B301" t="n">
+        <v>-0.06279478593825287</v>
       </c>
     </row>
   </sheetData>
@@ -445,7 +1885,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B2:B13"/>
+  <dimension ref="B2:B101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -455,62 +1895,502 @@
   <sheetData>
     <row r="2">
       <c r="B2" t="n">
-        <v>-4.113432240848646</v>
+        <v>-0.3345481827094603</v>
       </c>
     </row>
     <row r="3">
       <c r="B3" t="n">
-        <v>-5.279847779978951</v>
+        <v>0.0105854732284582</v>
       </c>
     </row>
     <row r="4">
       <c r="B4" t="n">
-        <v>-2.705284924943499</v>
+        <v>0.8594281295004332</v>
       </c>
     </row>
     <row r="5">
       <c r="B5" t="n">
-        <v>2.31116141196879</v>
+        <v>0.5187734500706381</v>
       </c>
     </row>
     <row r="6">
       <c r="B6" t="n">
-        <v>3.735102659178044</v>
+        <v>-0.7471972734666851</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" t="n">
-        <v>-0.6295253984484008</v>
+        <v>0.5634049504415173</v>
       </c>
     </row>
     <row r="8">
       <c r="B8" t="n">
-        <v>2.055168323361752</v>
+        <v>-0.3013742852951875</v>
       </c>
     </row>
     <row r="9">
       <c r="B9" t="n">
-        <v>5.264573548876267</v>
+        <v>0.6141901206184007</v>
       </c>
     </row>
     <row r="10">
       <c r="B10" t="n">
-        <v>-2.640681145525788</v>
+        <v>0.8682584342902635</v>
       </c>
     </row>
     <row r="11">
       <c r="B11" t="n">
-        <v>0.3515525764434081</v>
+        <v>-0.5272716917977446</v>
       </c>
     </row>
     <row r="12">
       <c r="B12" t="n">
-        <v>0.4599179390374482</v>
+        <v>-1.007442236752396</v>
       </c>
     </row>
     <row r="13">
       <c r="B13" t="n">
-        <v>3.78341401002889</v>
+        <v>-0.3665356442121965</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="B14" t="n">
+        <v>0.2619719345295713</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="B15" t="n">
+        <v>0.1839504409006087</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="B16" t="n">
+        <v>-0.8900504176224773</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="B17" t="n">
+        <v>-0.4787468798065005</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="B18" t="n">
+        <v>0.6673388435901474</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="B19" t="n">
+        <v>-0.6602174887354531</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="B20" t="n">
+        <v>0.7461933909479614</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="B21" t="n">
+        <v>0.09139251922328823</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="B22" t="n">
+        <v>-0.7946077216540232</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="B23" t="n">
+        <v>-0.9962916507327684</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="B24" t="n">
+        <v>0.4355459594016339</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="B25" t="n">
+        <v>0.9355033113534728</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="B26" t="n">
+        <v>0.8814641572375358</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="B27" t="n">
+        <v>0.8463748477976678</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="B28" t="n">
+        <v>-0.2706505296457954</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="B29" t="n">
+        <v>0.7577154756008566</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="B30" t="n">
+        <v>0.8827626877017276</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="B31" t="n">
+        <v>0.5627329660833624</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="B32" t="n">
+        <v>-0.9675834466146742</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="B33" t="n">
+        <v>0.4278393489280882</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="B34" t="n">
+        <v>0.6909260877330813</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="B35" t="n">
+        <v>0.118455515075036</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="B36" t="n">
+        <v>0.9241629882285772</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="B37" t="n">
+        <v>0.2194249098746745</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="B38" t="n">
+        <v>0.7505844036447815</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="B39" t="n">
+        <v>-0.5419237728135944</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="B40" t="n">
+        <v>-0.5319573698058414</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="B41" t="n">
+        <v>0.2672559164268122</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="B42" t="n">
+        <v>-0.7313068101799614</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="B43" t="n">
+        <v>0.8397062153094282</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="B44" t="n">
+        <v>-0.7850629373186613</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="B45" t="n">
+        <v>-0.200181508605609</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="B46" t="n">
+        <v>0.1920524455153584</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="B47" t="n">
+        <v>-0.6270151037926235</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="B48" t="n">
+        <v>-0.5038400041305533</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="B49" t="n">
+        <v>-0.274774817441676</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="B50" t="n">
+        <v>0.1643351298498273</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="B51" t="n">
+        <v>0.5448214660603369</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="B52" t="n">
+        <v>0.206582379888486</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="B53" t="n">
+        <v>0.266667622381083</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="B54" t="n">
+        <v>0.6953345140288416</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="B55" t="n">
+        <v>0.5998708143330647</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="B56" t="n">
+        <v>-0.3721054193230963</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="B57" t="n">
+        <v>1.02717755301076</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="B58" t="n">
+        <v>-0.7751650503588505</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="B59" t="n">
+        <v>0.9663967471595863</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="B60" t="n">
+        <v>-0.3773095708874198</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="B61" t="n">
+        <v>-0.9395211447192608</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="B62" t="n">
+        <v>-0.8951266658855992</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="B63" t="n">
+        <v>-0.8377069886549748</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="B64" t="n">
+        <v>0.2193805857768185</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="B65" t="n">
+        <v>0.3561692187588769</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="B66" t="n">
+        <v>0.1027134801009607</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="B67" t="n">
+        <v>0.03190841725376989</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="B68" t="n">
+        <v>0.2107086128252354</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="B69" t="n">
+        <v>-0.4341704721101379</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="B70" t="n">
+        <v>0.709149133565239</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="B71" t="n">
+        <v>-0.9605640305532579</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="B72" t="n">
+        <v>0.8398848358198844</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="B73" t="n">
+        <v>-0.4949756422101582</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="B74" t="n">
+        <v>0.2722306524725577</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="B75" t="n">
+        <v>0.8178033135586119</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="B76" t="n">
+        <v>-0.02580646258852834</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="B77" t="n">
+        <v>0.4413498238597161</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="B78" t="n">
+        <v>-0.7056847345722329</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="B79" t="n">
+        <v>-0.4267018555298774</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="B80" t="n">
+        <v>0.3551248782067001</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="B81" t="n">
+        <v>0.1081899412878378</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="B82" t="n">
+        <v>-0.6409701949682307</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="B83" t="n">
+        <v>-1.03676584091225</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="B84" t="n">
+        <v>0.2047183108300356</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="B85" t="n">
+        <v>0.8629571374606873</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="B86" t="n">
+        <v>0.2876541026072465</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="B87" t="n">
+        <v>0.3080832751641862</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="B88" t="n">
+        <v>-0.8470915341153923</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="B89" t="n">
+        <v>-0.03433583840825162</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="B90" t="n">
+        <v>0.3617997461683671</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="B91" t="n">
+        <v>0.8361722282961432</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="B92" t="n">
+        <v>0.4938565884659587</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="B93" t="n">
+        <v>-1.030111399476557</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="B94" t="n">
+        <v>0.4406632628495102</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="B95" t="n">
+        <v>-0.7055090566096502</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="B96" t="n">
+        <v>-0.03755066944382499</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="B97" t="n">
+        <v>0.828409274043738</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="B98" t="n">
+        <v>0.6618202088790903</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="B99" t="n">
+        <v>-0.7368854801996045</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="B100" t="n">
+        <v>0.8327887017022305</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="B101" t="n">
+        <v>-0.2560214644857574</v>
       </c>
     </row>
   </sheetData>
@@ -534,52 +2414,52 @@
   <sheetData>
     <row r="2">
       <c r="B2" t="n">
-        <v>-3.177031925254926</v>
+        <v>-0.6245139884660623</v>
       </c>
     </row>
     <row r="3">
       <c r="B3" t="n">
-        <v>-3.602775776160787</v>
+        <v>-0.5262171671074769</v>
       </c>
     </row>
     <row r="4">
       <c r="B4" t="n">
-        <v>-1.157940412245744</v>
+        <v>-0.1583931032411919</v>
       </c>
     </row>
     <row r="5">
       <c r="B5" t="n">
-        <v>-2.072033720407979</v>
+        <v>0.4923046194797043</v>
       </c>
     </row>
     <row r="6">
       <c r="B6" t="n">
-        <v>-1.026537384018153</v>
+        <v>0.9969130332563529</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" t="n">
-        <v>-1.784017713873747</v>
+        <v>-0.8475698520663525</v>
       </c>
     </row>
     <row r="8">
       <c r="B8" t="n">
-        <v>-1.739882481575725</v>
+        <v>-0.09527363188724856</v>
       </c>
     </row>
     <row r="9">
       <c r="B9" t="n">
-        <v>-0.8913597516781989</v>
+        <v>0.6927919757820352</v>
       </c>
     </row>
     <row r="10">
       <c r="B10" t="n">
-        <v>-2.190692084501851</v>
+        <v>0.5494759831026937</v>
       </c>
     </row>
     <row r="11">
       <c r="B11" t="n">
-        <v>-2.531749278898328</v>
+        <v>0.304569075730531</v>
       </c>
     </row>
   </sheetData>

</xml_diff>